<commit_message>
updated backlog, changed formatting of index, working on schedule
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -1116,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,11 +1219,15 @@
       <c r="H3" s="28">
         <v>1</v>
       </c>
-      <c r="I3" s="29"/>
+      <c r="I3" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="J3" s="30">
         <v>2</v>
       </c>
-      <c r="K3" s="29"/>
+      <c r="K3" s="29">
+        <v>2</v>
+      </c>
       <c r="L3" s="54"/>
       <c r="M3" s="55"/>
       <c r="N3" s="56"/>
@@ -1281,11 +1285,15 @@
       <c r="H5" s="28">
         <v>3</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="J5" s="30">
         <v>1</v>
       </c>
-      <c r="K5" s="29"/>
+      <c r="K5" s="29">
+        <v>1</v>
+      </c>
       <c r="L5" s="54"/>
       <c r="M5" s="55"/>
       <c r="N5" s="56"/>
@@ -1311,11 +1319,15 @@
       <c r="H6" s="28">
         <v>4</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="J6" s="30">
         <v>1</v>
       </c>
-      <c r="K6" s="29"/>
+      <c r="K6" s="29">
+        <v>0.5</v>
+      </c>
       <c r="L6" s="54"/>
       <c r="M6" s="55"/>
       <c r="N6" s="56"/>
@@ -1628,7 +1640,7 @@
       </c>
       <c r="K18" s="13">
         <f>SUM(K2:K15)</f>
-        <v>0.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated Backlog as of 4/29
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\Desktop\Part2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Di3drich\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5670"/>
   </bookViews>
   <sheets>
     <sheet name="Project Backlog" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -1117,23 +1117,23 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" customWidth="1"/>
-    <col min="5" max="5" width="58.5546875" customWidth="1"/>
-    <col min="6" max="6" width="60.5546875" customWidth="1"/>
-    <col min="7" max="7" width="42.5546875" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" customWidth="1"/>
+    <col min="6" max="6" width="60.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24">
         <v>9</v>
       </c>
@@ -1189,16 +1189,20 @@
       <c r="H2" s="28">
         <v>0</v>
       </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="J2" s="30">
         <v>10</v>
       </c>
-      <c r="K2" s="29"/>
+      <c r="K2" s="29">
+        <v>10</v>
+      </c>
       <c r="L2" s="51"/>
       <c r="M2" s="52"/>
       <c r="N2" s="53"/>
     </row>
-    <row r="3" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24">
         <v>1</v>
       </c>
@@ -1232,7 +1236,7 @@
       <c r="M3" s="55"/>
       <c r="N3" s="56"/>
     </row>
-    <row r="4" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>2</v>
       </c>
@@ -1266,7 +1270,7 @@
       <c r="M4" s="55"/>
       <c r="N4" s="56"/>
     </row>
-    <row r="5" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>3</v>
       </c>
@@ -1298,7 +1302,7 @@
       <c r="M5" s="55"/>
       <c r="N5" s="56"/>
     </row>
-    <row r="6" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -1332,7 +1336,7 @@
       <c r="M6" s="55"/>
       <c r="N6" s="56"/>
     </row>
-    <row r="7" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>4</v>
       </c>
@@ -1360,7 +1364,7 @@
       <c r="M7" s="55"/>
       <c r="N7" s="56"/>
     </row>
-    <row r="8" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -1399,7 +1403,7 @@
       </c>
       <c r="N8" s="59"/>
     </row>
-    <row r="9" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>6</v>
       </c>
@@ -1420,16 +1424,20 @@
       <c r="H9" s="35">
         <v>7</v>
       </c>
-      <c r="I9" s="36"/>
+      <c r="I9" s="36" t="s">
+        <v>54</v>
+      </c>
       <c r="J9" s="37">
         <v>4</v>
       </c>
-      <c r="K9" s="36"/>
+      <c r="K9" s="36">
+        <v>1</v>
+      </c>
       <c r="L9" s="60"/>
       <c r="M9" s="61"/>
       <c r="N9" s="62"/>
     </row>
-    <row r="10" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -1463,7 +1471,7 @@
       <c r="M10" s="64"/>
       <c r="N10" s="65"/>
     </row>
-    <row r="11" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>12</v>
       </c>
@@ -1482,16 +1490,20 @@
       <c r="H11" s="35">
         <v>9</v>
       </c>
-      <c r="I11" s="36"/>
+      <c r="I11" s="36" t="s">
+        <v>54</v>
+      </c>
       <c r="J11" s="37">
         <v>8</v>
       </c>
-      <c r="K11" s="36"/>
+      <c r="K11" s="36">
+        <v>4</v>
+      </c>
       <c r="L11" s="63"/>
       <c r="M11" s="64"/>
       <c r="N11" s="65"/>
     </row>
-    <row r="12" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>10</v>
       </c>
@@ -1510,16 +1522,20 @@
       <c r="H12" s="35">
         <v>10</v>
       </c>
-      <c r="I12" s="36"/>
+      <c r="I12" s="36" t="s">
+        <v>54</v>
+      </c>
       <c r="J12" s="37">
         <v>6</v>
       </c>
-      <c r="K12" s="36"/>
+      <c r="K12" s="36">
+        <v>4</v>
+      </c>
       <c r="L12" s="63"/>
       <c r="M12" s="64"/>
       <c r="N12" s="65"/>
     </row>
-    <row r="13" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>11</v>
       </c>
@@ -1538,11 +1554,15 @@
       <c r="H13" s="35">
         <v>11</v>
       </c>
-      <c r="I13" s="36"/>
+      <c r="I13" s="36" t="s">
+        <v>54</v>
+      </c>
       <c r="J13" s="37">
         <v>2</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="36">
+        <v>2</v>
+      </c>
       <c r="L13" s="66">
         <f>SUM(J9:J13)</f>
         <v>21</v>
@@ -1552,7 +1572,7 @@
       </c>
       <c r="N13" s="68"/>
     </row>
-    <row r="14" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>13</v>
       </c>
@@ -1580,7 +1600,7 @@
       <c r="M14" s="46"/>
       <c r="N14" s="47"/>
     </row>
-    <row r="15" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>14</v>
       </c>
@@ -1599,11 +1619,15 @@
       <c r="H15" s="42">
         <v>13</v>
       </c>
-      <c r="I15" s="43"/>
+      <c r="I15" s="43" t="s">
+        <v>54</v>
+      </c>
       <c r="J15" s="44">
         <v>8</v>
       </c>
-      <c r="K15" s="43"/>
+      <c r="K15" s="43">
+        <v>4</v>
+      </c>
       <c r="L15" s="48">
         <f>SUM(J14:J15)</f>
         <v>16</v>
@@ -1613,7 +1637,7 @@
       </c>
       <c r="N15" s="50"/>
     </row>
-    <row r="16" spans="1:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="69"/>
       <c r="B16" s="69"/>
       <c r="C16" s="69"/>
@@ -1626,7 +1650,7 @@
       <c r="J16" s="69"/>
       <c r="K16" s="19"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="20"/>
       <c r="H17" s="13"/>
@@ -1634,7 +1658,7 @@
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="20" t="s">
         <v>11</v>
@@ -1648,17 +1672,17 @@
       </c>
       <c r="K18" s="13">
         <f>SUM(K2:K15)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="20"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="20"/>
       <c r="G20" s="14"/>
@@ -1671,7 +1695,7 @@
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="20"/>
       <c r="G21" s="14"/>
@@ -1680,7 +1704,7 @@
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="20"/>
       <c r="E22" s="21"/>
@@ -1715,17 +1739,17 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" customWidth="1"/>
-    <col min="5" max="5" width="66.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="66.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1748,7 +1772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1771,7 +1795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1794,7 +1818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1815,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1836,7 +1860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1859,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1882,7 +1906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1905,7 +1929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1928,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1951,7 +1975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1972,7 +1996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1993,7 +2017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2014,7 +2038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2035,7 +2059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2056,7 +2080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F17" s="12" t="s">
         <v>52</v>
       </c>
@@ -2065,11 +2089,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19" s="14" t="s">
         <v>50</v>
       </c>
@@ -2078,12 +2102,12 @@
       </c>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20" s="14"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21" s="14" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
added group photo and updated backlog
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Di3drich\Desktop\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676"/>
   </bookViews>
   <sheets>
     <sheet name="Project Backlog" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -1114,26 +1114,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="58.5703125" customWidth="1"/>
-    <col min="6" max="6" width="60.5703125" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="58.5546875" customWidth="1"/>
+    <col min="6" max="6" width="60.5546875" customWidth="1"/>
+    <col min="7" max="7" width="42.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
         <v>9</v>
       </c>
@@ -1202,7 +1205,7 @@
       <c r="M2" s="52"/>
       <c r="N2" s="53"/>
     </row>
-    <row r="3" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24">
         <v>1</v>
       </c>
@@ -1236,7 +1239,7 @@
       <c r="M3" s="55"/>
       <c r="N3" s="56"/>
     </row>
-    <row r="4" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24">
         <v>2</v>
       </c>
@@ -1270,7 +1273,7 @@
       <c r="M4" s="55"/>
       <c r="N4" s="56"/>
     </row>
-    <row r="5" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
         <v>3</v>
       </c>
@@ -1302,7 +1305,7 @@
       <c r="M5" s="55"/>
       <c r="N5" s="56"/>
     </row>
-    <row r="6" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -1336,7 +1339,7 @@
       <c r="M6" s="55"/>
       <c r="N6" s="56"/>
     </row>
-    <row r="7" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24">
         <v>4</v>
       </c>
@@ -1355,16 +1358,20 @@
       <c r="H7" s="28">
         <v>5</v>
       </c>
-      <c r="I7" s="29"/>
+      <c r="I7" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="J7" s="30">
         <v>2</v>
       </c>
-      <c r="K7" s="29"/>
+      <c r="K7" s="29">
+        <v>1</v>
+      </c>
       <c r="L7" s="54"/>
       <c r="M7" s="55"/>
       <c r="N7" s="56"/>
     </row>
-    <row r="8" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -1403,7 +1410,7 @@
       </c>
       <c r="N8" s="59"/>
     </row>
-    <row r="9" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31">
         <v>6</v>
       </c>
@@ -1437,7 +1444,7 @@
       <c r="M9" s="61"/>
       <c r="N9" s="62"/>
     </row>
-    <row r="10" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -1471,7 +1478,7 @@
       <c r="M10" s="64"/>
       <c r="N10" s="65"/>
     </row>
-    <row r="11" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="31">
         <v>12</v>
       </c>
@@ -1503,7 +1510,7 @@
       <c r="M11" s="64"/>
       <c r="N11" s="65"/>
     </row>
-    <row r="12" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="31">
         <v>10</v>
       </c>
@@ -1535,7 +1542,7 @@
       <c r="M12" s="64"/>
       <c r="N12" s="65"/>
     </row>
-    <row r="13" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31">
         <v>11</v>
       </c>
@@ -1572,7 +1579,7 @@
       </c>
       <c r="N13" s="68"/>
     </row>
-    <row r="14" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38">
         <v>13</v>
       </c>
@@ -1591,16 +1598,20 @@
       <c r="H14" s="42">
         <v>12</v>
       </c>
-      <c r="I14" s="43"/>
+      <c r="I14" s="43" t="s">
+        <v>54</v>
+      </c>
       <c r="J14" s="44">
         <v>8</v>
       </c>
-      <c r="K14" s="43"/>
+      <c r="K14" s="43">
+        <v>16</v>
+      </c>
       <c r="L14" s="45"/>
       <c r="M14" s="46"/>
       <c r="N14" s="47"/>
     </row>
-    <row r="15" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="38">
         <v>14</v>
       </c>
@@ -1637,7 +1648,7 @@
       </c>
       <c r="N15" s="50"/>
     </row>
-    <row r="16" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="69"/>
       <c r="B16" s="69"/>
       <c r="C16" s="69"/>
@@ -1650,7 +1661,7 @@
       <c r="J16" s="69"/>
       <c r="K16" s="19"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="20"/>
       <c r="H17" s="13"/>
@@ -1658,7 +1669,7 @@
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="20" t="s">
         <v>11</v>
@@ -1672,17 +1683,17 @@
       </c>
       <c r="K18" s="13">
         <f>SUM(K2:K15)</f>
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="20"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="20"/>
       <c r="G20" s="14"/>
@@ -1695,7 +1706,7 @@
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="20"/>
       <c r="G21" s="14"/>
@@ -1704,7 +1715,7 @@
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="20"/>
       <c r="E22" s="21"/>
@@ -1727,7 +1738,8 @@
     <mergeCell ref="A16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="39" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1739,17 +1751,17 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="66.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" customWidth="1"/>
+    <col min="5" max="5" width="66.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1772,7 +1784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1795,7 +1807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1818,7 +1830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1839,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1860,7 +1872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1883,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1906,7 +1918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1929,7 +1941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1952,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1975,7 +1987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1996,7 +2008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -2017,7 +2029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2038,7 +2050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2059,7 +2071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
       <c r="F17" s="12" t="s">
         <v>52</v>
       </c>
@@ -2089,11 +2101,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E19" s="14" t="s">
         <v>50</v>
       </c>
@@ -2102,12 +2114,12 @@
       </c>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E20" s="14"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E21" s="14" t="s">
         <v>51</v>
       </c>

</xml_diff>